<commit_message>
Add Streamlit app and initial files
</commit_message>
<xml_diff>
--- a/Values.xlsx
+++ b/Values.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymos\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymos\Documents\TKF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1486D608-AD0E-417B-B3F6-5E658ACEDBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ED1237-777E-4B75-BAA6-0F3D4CE3F4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Datum</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Aluminum Gloeier pH Waarde</t>
+  </si>
+  <si>
+    <t>Medewerker</t>
   </si>
   <si>
     <t>2024-10-01</t>
@@ -507,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,10 +546,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>14.7</v>
@@ -573,9 +579,9 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>15.9</v>
@@ -602,9 +608,9 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>15.5</v>
@@ -631,9 +637,9 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>15.2</v>
@@ -660,9 +666,9 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>14.3</v>
@@ -689,9 +695,9 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>14.3</v>
@@ -718,9 +724,9 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>14.1</v>
@@ -747,9 +753,9 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>15.7</v>
@@ -776,9 +782,9 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>15.2</v>
@@ -805,9 +811,9 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>15.4</v>
@@ -834,9 +840,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>14</v>
@@ -863,9 +869,9 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>15.9</v>
@@ -892,9 +898,9 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>15.7</v>
@@ -921,9 +927,9 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>14.4</v>
@@ -950,9 +956,9 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>14.4</v>
@@ -981,7 +987,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>14.4</v>
@@ -1010,7 +1016,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>14.6</v>
@@ -1039,7 +1045,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19">
         <v>15</v>
@@ -1068,7 +1074,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>14.9</v>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>14.6</v>
@@ -1126,7 +1132,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>15.2</v>
@@ -1155,7 +1161,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>14.3</v>
@@ -1184,7 +1190,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>14.6</v>
@@ -1213,7 +1219,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>14.7</v>
@@ -1242,7 +1248,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>14.9</v>
@@ -1271,7 +1277,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>15.6</v>
@@ -1300,7 +1306,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>14.4</v>
@@ -1329,7 +1335,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>15</v>
@@ -1358,7 +1364,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30">
         <v>15.2</v>
@@ -1387,7 +1393,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31">
         <v>14.1</v>
@@ -1416,7 +1422,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32">
         <v>15.2</v>

</xml_diff>